<commit_message>
changed interface to generate report, added date; Also added FX.xlsx to accomodate FX rates on different dates
</commit_message>
<xml_diff>
--- a/AssetType_SpecialCase.xlsx
+++ b/AssetType_SpecialCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\risk_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE02100-EBC8-4EF7-95CF-41358DE741FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D149F1-B68F-4282-B230-4E1C5A24EB8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33480" yWindow="195" windowWidth="21960" windowHeight="14850" xr2:uid="{ACE90E50-0C10-451E-84C3-1EA5214A7D62}"/>
+    <workbookView xWindow="32055" yWindow="150" windowWidth="21960" windowHeight="14850" xr2:uid="{ACE90E50-0C10-451E-84C3-1EA5214A7D62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>ID</t>
   </si>
@@ -41,27 +41,9 @@
     <t>AssetType</t>
   </si>
   <si>
-    <t>2823 HK Equity</t>
-  </si>
-  <si>
-    <t>HK</t>
-  </si>
-  <si>
-    <t>Fund, Real Estate Investment Trusts, SFC authorized</t>
-  </si>
-  <si>
-    <t>Fund, Exchange Traded Funds, SFC authorized</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>iShares A50 China ETF</t>
-  </si>
-  <si>
-    <t>LINK REITs</t>
-  </si>
-  <si>
     <t>Portfolio</t>
   </si>
   <si>
@@ -75,9 +57,6 @@
   </si>
   <si>
     <t>CN</t>
-  </si>
-  <si>
-    <t>823 HK Equity</t>
   </si>
   <si>
     <t>Equity, Listed equities</t>
@@ -153,7 +132,7 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4150880" cy="1125693"/>
+    <xdr:ext cx="4150880" cy="1470146"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1">
@@ -167,8 +146,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9277350" y="123825"/>
-          <a:ext cx="4150880" cy="1125693"/>
+          <a:off x="9334500" y="123825"/>
+          <a:ext cx="4150880" cy="1470146"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -212,7 +191,16 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>information, e.g., open ended fund or private security.</a:t>
+            <a:t>information, e.g., open ended fund or private security;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>2) For those that need to override the default asset type;</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -537,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E602E101-F235-4094-9FDA-0F669DCC6F01}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -558,13 +546,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -572,47 +560,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>19437</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
can build LQA combined master list now
</commit_message>
<xml_diff>
--- a/AssetType_SpecialCase.xlsx
+++ b/AssetType_SpecialCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\risk_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D149F1-B68F-4282-B230-4E1C5A24EB8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2A945A-3D25-4400-B9B3-4B107C878597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32055" yWindow="150" windowWidth="21960" windowHeight="14850" xr2:uid="{ACE90E50-0C10-451E-84C3-1EA5214A7D62}"/>
+    <workbookView xWindow="4770" yWindow="255" windowWidth="21960" windowHeight="14850" xr2:uid="{ACE90E50-0C10-451E-84C3-1EA5214A7D62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>ID</t>
   </si>
@@ -60,6 +60,21 @@
   </si>
   <si>
     <t>Equity, Listed equities</t>
+  </si>
+  <si>
+    <t>823 HK Equity</t>
+  </si>
+  <si>
+    <t>6823 HK Equity</t>
+  </si>
+  <si>
+    <t>LINK REITs</t>
+  </si>
+  <si>
+    <t>HK</t>
+  </si>
+  <si>
+    <t>HKT Trust and HKT Ltd</t>
   </si>
 </sst>
 </file>
@@ -525,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E602E101-F235-4094-9FDA-0F669DCC6F01}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -575,6 +590,34 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
did 20051 asset allocation
</commit_message>
<xml_diff>
--- a/AssetType_SpecialCase.xlsx
+++ b/AssetType_SpecialCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\risk_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2A945A-3D25-4400-B9B3-4B107C878597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1233BD30-A7AC-4A6D-A696-991FCBA5220D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4770" yWindow="255" windowWidth="21960" windowHeight="14850" xr2:uid="{ACE90E50-0C10-451E-84C3-1EA5214A7D62}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ACE90E50-0C10-451E-84C3-1EA5214A7D62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -75,6 +75,21 @@
   </si>
   <si>
     <t>HKT Trust and HKT Ltd</t>
+  </si>
+  <si>
+    <t>.FSFUND HK Equity</t>
+  </si>
+  <si>
+    <t>First SeaFront Fund</t>
+  </si>
+  <si>
+    <t>Fund, Other Funds</t>
+  </si>
+  <si>
+    <t>CLFLDIF HK Equity</t>
+  </si>
+  <si>
+    <t>Diversified Income Fund</t>
   </si>
 </sst>
 </file>
@@ -540,16 +555,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E602E101-F235-4094-9FDA-0F669DCC6F01}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="11.25" customWidth="1"/>
     <col min="4" max="4" width="13.75" customWidth="1"/>
     <col min="5" max="5" width="46.375" customWidth="1"/>
@@ -618,6 +633,34 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
just generated asset allocation for all portfolios across the company
</commit_message>
<xml_diff>
--- a/AssetType_SpecialCase.xlsx
+++ b/AssetType_SpecialCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\risk_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1233BD30-A7AC-4A6D-A696-991FCBA5220D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7BF7EA-BF8C-4DF3-8D6E-F701600D127D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ACE90E50-0C10-451E-84C3-1EA5214A7D62}"/>
+    <workbookView xWindow="30090" yWindow="510" windowWidth="21960" windowHeight="14850" xr2:uid="{ACE90E50-0C10-451E-84C3-1EA5214A7D62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -90,6 +90,66 @@
   </si>
   <si>
     <t>Diversified Income Fund</t>
+  </si>
+  <si>
+    <t>ICSUSPI ID Equity</t>
+  </si>
+  <si>
+    <t>BlackRock ICS US Dollar Liquidity Fund</t>
+  </si>
+  <si>
+    <t>Global Fund?</t>
+  </si>
+  <si>
+    <t>Fixed Income, Cash equivalents</t>
+  </si>
+  <si>
+    <t>JPMULCD LX Equity</t>
+  </si>
+  <si>
+    <t>JPMorgan Liquidity Funds</t>
+  </si>
+  <si>
+    <t>QQQ US Equity</t>
+  </si>
+  <si>
+    <t>Fund, Exchange Traded Funds</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Investco QQQ Trust Series 1</t>
+  </si>
+  <si>
+    <t>USG8116KAB82</t>
+  </si>
+  <si>
+    <t>SHNTN 2015-1X B</t>
+  </si>
+  <si>
+    <t>Fixed income, Asset-Backed, Cash</t>
+  </si>
+  <si>
+    <t>Country not sure, is it Cash or Synthetic?</t>
+  </si>
+  <si>
+    <t>SPY US Equity</t>
+  </si>
+  <si>
+    <t>SPDR S&amp;P 500 ETF Trust</t>
+  </si>
+  <si>
+    <t>2823 HK Equity</t>
+  </si>
+  <si>
+    <t>2828 HK Equity</t>
+  </si>
+  <si>
+    <t>iShares FTSE A50 China ETF</t>
+  </si>
+  <si>
+    <t>Hang Seng China Enterprises Index ETF</t>
   </si>
 </sst>
 </file>
@@ -113,12 +173,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -133,9 +199,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,23 +622,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E602E101-F235-4094-9FDA-0F669DCC6F01}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="1" max="1" width="16.75" customWidth="1"/>
+    <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.25" customWidth="1"/>
     <col min="4" max="4" width="13.75" customWidth="1"/>
-    <col min="5" max="5" width="46.375" customWidth="1"/>
+    <col min="5" max="5" width="29.75" customWidth="1"/>
     <col min="6" max="6" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -588,7 +655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -605,60 +672,170 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test case for 20200630 and 20200930 liquidity and asset allocation numbers.
</commit_message>
<xml_diff>
--- a/AssetType_SpecialCase.xlsx
+++ b/AssetType_SpecialCase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\risk_report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhangst\git\risk_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7BF7EA-BF8C-4DF3-8D6E-F701600D127D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC72343-6AE0-4236-98CE-7AE9AA6DB721}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30090" yWindow="510" windowWidth="21960" windowHeight="14850" xr2:uid="{ACE90E50-0C10-451E-84C3-1EA5214A7D62}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{ACE90E50-0C10-451E-84C3-1EA5214A7D62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -150,6 +150,21 @@
   </si>
   <si>
     <t>Hang Seng China Enterprises Index ETF</t>
+  </si>
+  <si>
+    <t>XS2166383799</t>
+  </si>
+  <si>
+    <t>APICORP (SuperNational Corporation)</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>Fixed Income, Government / Municipal</t>
+  </si>
+  <si>
+    <t>Supernational in Saudi Arabia, use country of domicile as proxy i.e. SA (or Saudi Arabia)</t>
   </si>
 </sst>
 </file>
@@ -199,10 +214,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,23 +638,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E602E101-F235-4094-9FDA-0F669DCC6F01}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.75" customWidth="1"/>
+    <col min="1" max="1" width="16.69921875" customWidth="1"/>
     <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.25" customWidth="1"/>
-    <col min="4" max="4" width="13.75" customWidth="1"/>
-    <col min="5" max="5" width="29.75" customWidth="1"/>
-    <col min="6" max="6" width="13.125" customWidth="1"/>
+    <col min="3" max="3" width="11.19921875" customWidth="1"/>
+    <col min="4" max="4" width="13.69921875" customWidth="1"/>
+    <col min="5" max="5" width="34.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -655,7 +671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -672,7 +688,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -686,7 +702,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -700,7 +716,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -714,7 +730,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -728,7 +744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -742,7 +758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -756,7 +772,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -773,7 +789,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -790,7 +806,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -804,7 +820,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -824,7 +840,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -836,6 +852,23 @@
       </c>
       <c r="E13" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>